<commit_message>
Extreme trial egg laying data.
</commit_message>
<xml_diff>
--- a/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/mother_laying_bydate.xlsx
+++ b/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/mother_laying_bydate.xlsx
@@ -8,27 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/SBB-dispersal/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAD55D8-93CE-6C47-A884-297295CABEEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9059D8-0DF3-594A-A7B3-121D08B94898}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{E14F8870-8DED-064C-A3A0-F7635F8AECA1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="mother_laying_bydate" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$E$2:$E$30</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$F$2:$F$30</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$F$2:$F$30</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$2:$E$30</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$F$2:$F$30</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$2:$E$30</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$F$2:$F$30</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$E$2:$E$30</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="15">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="17">
   <si>
     <t>collect_date</t>
   </si>
@@ -84,6 +67,15 @@
   </si>
   <si>
     <t>HS</t>
+  </si>
+  <si>
+    <t>8.27.21</t>
+  </si>
+  <si>
+    <t>LW</t>
+  </si>
+  <si>
+    <t>MID</t>
   </si>
 </sst>
 </file>
@@ -435,29 +427,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE6B1BE-B14C-BE4C-BCD4-C1716963499F}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -465,13 +455,13 @@
         <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -479,13 +469,13 @@
         <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -493,13 +483,13 @@
         <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -507,13 +497,13 @@
         <v>335</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -521,13 +511,13 @@
         <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -535,13 +525,13 @@
         <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -549,13 +539,13 @@
         <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -563,13 +553,13 @@
         <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -577,13 +567,13 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -591,13 +581,13 @@
         <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -605,13 +595,13 @@
         <v>211</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -619,13 +609,13 @@
         <v>118</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -633,13 +623,13 @@
         <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -647,13 +637,13 @@
         <v>329</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -661,13 +651,13 @@
         <v>363</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -675,13 +665,13 @@
         <v>335</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -689,13 +679,13 @@
         <v>262</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -703,13 +693,13 @@
         <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19">
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -717,13 +707,13 @@
         <v>164</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -731,13 +721,13 @@
         <v>339</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21">
         <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -745,13 +735,13 @@
         <v>389</v>
       </c>
       <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
         <v>12</v>
-      </c>
-      <c r="C22">
-        <v>14</v>
-      </c>
-      <c r="E22" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -759,13 +749,13 @@
         <v>367</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23">
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -773,13 +763,13 @@
         <v>288</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24">
         <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -787,13 +777,13 @@
         <v>387</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -801,13 +791,13 @@
         <v>349</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C26">
         <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -815,13 +805,13 @@
         <v>355</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C27">
         <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -829,13 +819,13 @@
         <v>229</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28">
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -843,13 +833,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29">
         <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -857,13 +847,433 @@
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30">
         <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>119</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>211</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>83</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>118</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34">
+        <v>40</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>288</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>298</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>329</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <v>92</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>316</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39">
+        <v>17</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40">
+        <v>19</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>73</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <v>26</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42">
+        <v>29</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>317</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43">
+        <v>16</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>103</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>104</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>363</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>263</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <v>31</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>153</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48">
+        <v>18</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>247</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>61</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50">
+        <v>14</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>355</v>
+      </c>
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51">
+        <v>8</v>
+      </c>
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>24</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52">
+        <v>10</v>
+      </c>
+      <c r="E52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>356</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53">
+        <v>20</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>232</v>
+      </c>
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54">
+        <v>33</v>
+      </c>
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>33</v>
+      </c>
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55">
+        <v>35</v>
+      </c>
+      <c r="E55" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>348</v>
+      </c>
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56">
+        <v>22</v>
+      </c>
+      <c r="E56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>129</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57">
+        <v>21</v>
+      </c>
+      <c r="E57" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>41</v>
+      </c>
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58">
+        <v>44</v>
+      </c>
+      <c r="E58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>29</v>
+      </c>
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59">
+        <v>14</v>
+      </c>
+      <c r="E59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>22</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Egg laying datasheet finished.
</commit_message>
<xml_diff>
--- a/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/mother_laying_bydate.xlsx
+++ b/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/mother_laying_bydate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/SBB-dispersal/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C43181-B3A7-6F4C-B890-1F4A086D8A87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F74171-A083-C84F-A44C-4D3720B815F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{E14F8870-8DED-064C-A3A0-F7635F8AECA1}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{E14F8870-8DED-064C-A3A0-F7635F8AECA1}"/>
   </bookViews>
   <sheets>
     <sheet name="mother_laying_bydate" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="25">
   <si>
     <t>collect_date</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>10.07.21</t>
+  </si>
+  <si>
+    <t>10.18.21</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE6B1BE-B14C-BE4C-BCD4-C1716963499F}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2925,6 +2928,193 @@
         <v>7</v>
       </c>
     </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>114</v>
+      </c>
+      <c r="B167" t="s">
+        <v>24</v>
+      </c>
+      <c r="C167">
+        <v>18</v>
+      </c>
+      <c r="D167">
+        <v>4</v>
+      </c>
+      <c r="E167" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>118</v>
+      </c>
+      <c r="B168" t="s">
+        <v>24</v>
+      </c>
+      <c r="C168">
+        <v>21</v>
+      </c>
+      <c r="D168">
+        <v>0</v>
+      </c>
+      <c r="E168" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>329</v>
+      </c>
+      <c r="B169" t="s">
+        <v>24</v>
+      </c>
+      <c r="C169">
+        <v>24</v>
+      </c>
+      <c r="D169">
+        <v>0</v>
+      </c>
+      <c r="E169" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>103</v>
+      </c>
+      <c r="B170" t="s">
+        <v>24</v>
+      </c>
+      <c r="C170">
+        <v>10</v>
+      </c>
+      <c r="D170">
+        <v>0</v>
+      </c>
+      <c r="E170" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>335</v>
+      </c>
+      <c r="B171" t="s">
+        <v>24</v>
+      </c>
+      <c r="C171">
+        <v>4</v>
+      </c>
+      <c r="D171">
+        <v>4</v>
+      </c>
+      <c r="E171" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>202</v>
+      </c>
+      <c r="B172" t="s">
+        <v>24</v>
+      </c>
+      <c r="C172">
+        <v>2</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>339</v>
+      </c>
+      <c r="B173" t="s">
+        <v>24</v>
+      </c>
+      <c r="C173">
+        <v>27</v>
+      </c>
+      <c r="D173">
+        <v>3</v>
+      </c>
+      <c r="E173" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>211</v>
+      </c>
+      <c r="B174" t="s">
+        <v>24</v>
+      </c>
+      <c r="C174">
+        <v>6</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>317</v>
+      </c>
+      <c r="B175" t="s">
+        <v>24</v>
+      </c>
+      <c r="C175">
+        <v>36</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>16</v>
+      </c>
+      <c r="B176" t="s">
+        <v>24</v>
+      </c>
+      <c r="C176">
+        <v>98</v>
+      </c>
+      <c r="D176">
+        <v>12</v>
+      </c>
+      <c r="E176" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>339</v>
+      </c>
+      <c r="B177" t="s">
+        <v>24</v>
+      </c>
+      <c r="C177">
+        <v>42</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>